<commit_message>
Updated formulas and added .gitignore items.
</commit_message>
<xml_diff>
--- a/Jones_2019.xlsx
+++ b/Jones_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F152AC30-B738-4341-BCD8-1D8D4C69B9EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD62D96B-D717-4F2E-879A-AE33CF85C10E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7950" yWindow="4560" windowWidth="28800" windowHeight="15472" xr2:uid="{608B4A5A-17A8-425D-B6FD-CBB618A13900}"/>
+    <workbookView xWindow="21225" yWindow="2625" windowWidth="17100" windowHeight="15908" xr2:uid="{608B4A5A-17A8-425D-B6FD-CBB618A13900}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="1" r:id="rId1"/>
@@ -131,6 +131,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,8 +163,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +483,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -508,7 +512,8 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
+        <f>Student_1!B3</f>
         <v>87.5</v>
       </c>
     </row>
@@ -522,7 +527,8 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
+        <f>Student_2!B3</f>
         <v>90.3</v>
       </c>
     </row>
@@ -536,7 +542,8 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
+        <f>Student_3!B3</f>
         <v>82.3</v>
       </c>
     </row>
@@ -550,7 +557,8 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
+        <f>Student_4!B3</f>
         <v>90.6</v>
       </c>
     </row>
@@ -564,7 +572,8 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
+        <f>Student_5!B3</f>
         <v>88.4</v>
       </c>
     </row>
@@ -578,7 +587,8 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
+        <f>Student_6!B3</f>
         <v>88.7</v>
       </c>
     </row>
@@ -592,12 +602,16 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
+        <f>Student_7!B3</f>
         <v>86.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -606,7 +620,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>